<commit_message>
fl csvs/stom data updates
</commit_message>
<xml_diff>
--- a/data/Experiment/Raw/StomatalDensity.xlsx
+++ b/data/Experiment/Raw/StomatalDensity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/SeedlingMortality/data/Experiment/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D2A1FE-B069-AC49-B7D9-A605615C6040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4894DDED-DA6B-C047-BDEE-F0B2878DF07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23600" windowHeight="17120" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="244">
   <si>
     <t>PIPO1</t>
   </si>
@@ -819,7 +819,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -827,15 +827,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F958DE17-0E59-E849-A835-10176DABDFD5}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1262,7 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D67" si="0">C5/B5</f>
+        <f t="shared" ref="D5:D69" si="0">C5/B5</f>
         <v>59.382422802850357</v>
       </c>
     </row>
@@ -1326,7 +1337,7 @@
         <v>49</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10" si="2">C10/B10</f>
+        <f t="shared" ref="D10:D12" si="2">C10/B10</f>
         <v>61.25</v>
       </c>
     </row>
@@ -1334,41 +1345,59 @@
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B11">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="C11">
+        <v>74</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11" si="3">C11/B11</f>
+        <v>46.365914786967416</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="C12">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>66.326530612244895</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="e">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>44.900577293136628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" t="e">
         <f t="shared" si="0"/>
@@ -1377,7 +1406,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" t="e">
         <f t="shared" si="0"/>
@@ -1386,7 +1415,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D17" t="e">
         <f t="shared" si="0"/>
@@ -1395,7 +1424,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18" t="e">
         <f t="shared" si="0"/>
@@ -1404,7 +1433,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19" t="e">
         <f t="shared" si="0"/>
@@ -1413,7 +1442,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D20" t="e">
         <f t="shared" si="0"/>
@@ -1422,7 +1451,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D21" t="e">
         <f t="shared" si="0"/>
@@ -1431,7 +1460,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22" t="e">
         <f t="shared" si="0"/>
@@ -1440,7 +1469,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23" t="e">
         <f t="shared" si="0"/>
@@ -1449,7 +1478,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24" t="e">
         <f t="shared" si="0"/>
@@ -1458,7 +1487,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D25" t="e">
         <f t="shared" si="0"/>
@@ -1467,7 +1496,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D26" t="e">
         <f t="shared" si="0"/>
@@ -1476,7 +1505,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D27" t="e">
         <f t="shared" si="0"/>
@@ -1485,7 +1514,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D28" t="e">
         <f t="shared" si="0"/>
@@ -1494,7 +1523,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D29" t="e">
         <f t="shared" si="0"/>
@@ -1503,7 +1532,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D30" t="e">
         <f t="shared" si="0"/>
@@ -1512,7 +1541,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D31" t="e">
         <f t="shared" si="0"/>
@@ -1521,7 +1550,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D32" t="e">
         <f t="shared" si="0"/>
@@ -1530,7 +1559,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D33" t="e">
         <f t="shared" si="0"/>
@@ -1539,7 +1568,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34" t="e">
         <f t="shared" si="0"/>
@@ -1548,7 +1577,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D35" t="e">
         <f t="shared" si="0"/>
@@ -1557,7 +1586,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D36" t="e">
         <f t="shared" si="0"/>
@@ -1566,25 +1595,25 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D37" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D39" t="e">
         <f t="shared" si="0"/>
@@ -1593,7 +1622,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D40" t="e">
         <f t="shared" si="0"/>
@@ -1602,7 +1631,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D41" t="e">
         <f t="shared" si="0"/>
@@ -1611,7 +1640,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D42" t="e">
         <f t="shared" si="0"/>
@@ -1620,7 +1649,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D43" t="e">
         <f t="shared" si="0"/>
@@ -1629,7 +1658,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D44" t="e">
         <f t="shared" si="0"/>
@@ -1638,7 +1667,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D45" t="e">
         <f t="shared" si="0"/>
@@ -1647,7 +1676,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D46" t="e">
         <f t="shared" si="0"/>
@@ -1656,7 +1685,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D47" t="e">
         <f t="shared" si="0"/>
@@ -1665,7 +1694,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D48" t="e">
         <f t="shared" si="0"/>
@@ -1674,7 +1703,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D49" t="e">
         <f t="shared" si="0"/>
@@ -1683,7 +1712,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D50" t="e">
         <f t="shared" si="0"/>
@@ -1692,7 +1721,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D51" t="e">
         <f t="shared" si="0"/>
@@ -1701,7 +1730,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D52" t="e">
         <f t="shared" si="0"/>
@@ -1710,7 +1739,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D53" t="e">
         <f t="shared" si="0"/>
@@ -1719,7 +1748,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D54" t="e">
         <f t="shared" si="0"/>
@@ -1728,7 +1757,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D55" t="e">
         <f t="shared" si="0"/>
@@ -1737,7 +1766,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D56" t="e">
         <f t="shared" si="0"/>
@@ -1746,7 +1775,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D57" t="e">
         <f t="shared" si="0"/>
@@ -1755,7 +1784,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D58" t="e">
         <f t="shared" si="0"/>
@@ -1764,7 +1793,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D59" t="e">
         <f t="shared" si="0"/>
@@ -1773,7 +1802,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D60" t="e">
         <f t="shared" si="0"/>
@@ -1782,7 +1811,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D61" t="e">
         <f t="shared" si="0"/>
@@ -1791,7 +1820,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D62" t="e">
         <f t="shared" si="0"/>
@@ -1800,7 +1829,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D63" t="e">
         <f t="shared" si="0"/>
@@ -1809,7 +1838,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D64" t="e">
         <f t="shared" si="0"/>
@@ -1818,7 +1847,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D65" t="e">
         <f t="shared" si="0"/>
@@ -1827,7 +1856,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D66" t="e">
         <f t="shared" si="0"/>
@@ -1836,9 +1865,27 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D68" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D67" t="e">
+      <c r="D69" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
week 4 day 4 ... partially
</commit_message>
<xml_diff>
--- a/data/Experiment/Raw/StomatalDensity.xlsx
+++ b/data/Experiment/Raw/StomatalDensity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/SeedlingMortality/data/Experiment/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4894DDED-DA6B-C047-BDEE-F0B2878DF07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1BB8D4-FBF1-6344-A45C-357631DECE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23600" windowHeight="17120" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="244">
   <si>
     <t>PIPO1</t>
   </si>
@@ -819,7 +819,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -827,26 +827,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,10 +1174,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F958DE17-0E59-E849-A835-10176DABDFD5}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1201,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -1222,7 +1216,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B3">
@@ -1237,7 +1231,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B4">
@@ -1252,7 +1246,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B5">
@@ -1262,12 +1256,12 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D69" si="0">C5/B5</f>
+        <f t="shared" ref="D5:D75" si="0">C5/B5</f>
         <v>59.382422802850357</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B6">
@@ -1282,7 +1276,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7">
@@ -1297,7 +1291,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B8">
@@ -1312,7 +1306,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B9">
@@ -1327,7 +1321,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B10">
@@ -1342,7 +1336,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B11">
@@ -1357,7 +1351,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B12">
@@ -1372,7 +1366,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B13">
@@ -1386,90 +1380,144 @@
         <v>44.900577293136628</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="4">
+        <v>1.657</v>
+      </c>
+      <c r="C14" s="4">
+        <v>79</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>47.676523838261922</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="C15" s="5">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" ref="D15" si="4">C15/B15</f>
+        <v>46.793760831889088</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.495</v>
+      </c>
+      <c r="C16" s="5">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>50.505050505050505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="B17" s="5">
+        <v>2.4630000000000001</v>
+      </c>
+      <c r="C17" s="5">
+        <v>105</v>
+      </c>
+      <c r="D17">
+        <f>C17/B17</f>
+        <v>42.630937880633375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="C18" s="5">
+        <v>42</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18" si="5">C18/B18</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C19" s="5">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>56.930693069306926</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B20" s="5">
+        <v>1.7270000000000001</v>
+      </c>
+      <c r="C20" s="5">
+        <v>71</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>41.111754487550662</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="C21" s="5">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21" si="6">C21/B21</f>
+        <v>38.878842676311031</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>45.714285714285715</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D23" t="e">
         <f t="shared" si="0"/>
@@ -1478,7 +1526,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D24" t="e">
         <f t="shared" si="0"/>
@@ -1487,7 +1535,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D25" t="e">
         <f t="shared" si="0"/>
@@ -1496,7 +1544,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D26" t="e">
         <f t="shared" si="0"/>
@@ -1505,7 +1553,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D27" t="e">
         <f t="shared" si="0"/>
@@ -1514,7 +1562,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D28" t="e">
         <f t="shared" si="0"/>
@@ -1523,7 +1571,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D29" t="e">
         <f t="shared" si="0"/>
@@ -1532,7 +1580,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D30" t="e">
         <f t="shared" si="0"/>
@@ -1541,7 +1589,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D31" t="e">
         <f t="shared" si="0"/>
@@ -1550,7 +1598,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D32" t="e">
         <f t="shared" si="0"/>
@@ -1559,7 +1607,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D33" t="e">
         <f t="shared" si="0"/>
@@ -1568,7 +1616,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D34" t="e">
         <f t="shared" si="0"/>
@@ -1577,7 +1625,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D35" t="e">
         <f t="shared" si="0"/>
@@ -1586,7 +1634,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D36" t="e">
         <f t="shared" si="0"/>
@@ -1595,7 +1643,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D37" t="e">
         <f t="shared" si="0"/>
@@ -1604,7 +1652,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D38" t="e">
         <f t="shared" si="0"/>
@@ -1613,61 +1661,61 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D45" t="e">
         <f t="shared" si="0"/>
@@ -1676,7 +1724,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D46" t="e">
         <f t="shared" si="0"/>
@@ -1685,7 +1733,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D47" t="e">
         <f t="shared" si="0"/>
@@ -1694,7 +1742,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D48" t="e">
         <f t="shared" si="0"/>
@@ -1703,7 +1751,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D49" t="e">
         <f t="shared" si="0"/>
@@ -1712,7 +1760,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D50" t="e">
         <f t="shared" si="0"/>
@@ -1721,7 +1769,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D51" t="e">
         <f t="shared" si="0"/>
@@ -1730,7 +1778,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D52" t="e">
         <f t="shared" si="0"/>
@@ -1739,7 +1787,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D53" t="e">
         <f t="shared" si="0"/>
@@ -1748,7 +1796,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D54" t="e">
         <f t="shared" si="0"/>
@@ -1757,7 +1805,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D55" t="e">
         <f t="shared" si="0"/>
@@ -1766,7 +1814,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D56" t="e">
         <f t="shared" si="0"/>
@@ -1775,7 +1823,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D57" t="e">
         <f t="shared" si="0"/>
@@ -1784,7 +1832,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D58" t="e">
         <f t="shared" si="0"/>
@@ -1793,7 +1841,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D59" t="e">
         <f t="shared" si="0"/>
@@ -1802,7 +1850,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D60" t="e">
         <f t="shared" si="0"/>
@@ -1811,7 +1859,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D61" t="e">
         <f t="shared" si="0"/>
@@ -1820,7 +1868,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D62" t="e">
         <f t="shared" si="0"/>
@@ -1829,7 +1877,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D63" t="e">
         <f t="shared" si="0"/>
@@ -1838,7 +1886,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D64" t="e">
         <f t="shared" si="0"/>
@@ -1847,7 +1895,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D65" t="e">
         <f t="shared" si="0"/>
@@ -1856,7 +1904,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D66" t="e">
         <f t="shared" si="0"/>
@@ -1865,7 +1913,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D67" t="e">
         <f t="shared" si="0"/>
@@ -1874,7 +1922,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D68" t="e">
         <f t="shared" si="0"/>
@@ -1883,9 +1931,63 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D71" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D72" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D74" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D69" t="e">
+      <c r="D75" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
moved some files/worked on stomata
</commit_message>
<xml_diff>
--- a/data/Experiment/Raw/StomatalDensity.xlsx
+++ b/data/Experiment/Raw/StomatalDensity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/SeedlingMortality/data/Experiment/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA8EF2A-D02E-7141-9B81-68D1DB7B4BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9212CDA-6C66-2544-BB01-DEF367E9492F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23600" windowHeight="17120" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22520" windowHeight="17120" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
   <sheets>
     <sheet name="PIPO" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="244">
   <si>
     <t>PIPO1</t>
   </si>
@@ -1171,11 +1171,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F958DE17-0E59-E849-A835-10176DABDFD5}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A47:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,7 +1253,7 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D87" si="0">C5/B5</f>
+        <f t="shared" ref="D5:D93" si="0">C5/B5</f>
         <v>59.382422802850357</v>
       </c>
     </row>
@@ -1738,116 +1738,188 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D38" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B38">
+        <v>1.732</v>
+      </c>
+      <c r="C38">
+        <v>91</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>52.540415704387989</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D39" t="e">
+      <c r="B39">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C39">
+        <v>47</v>
+      </c>
+      <c r="D39">
         <f t="shared" ref="D39" si="12">C39/B39</f>
-        <v>#DIV/0!</v>
+        <v>41.964285714285708</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D40" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B40">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>53.370786516853933</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D41" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B41">
+        <v>1.08</v>
+      </c>
+      <c r="C41">
+        <v>83</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>76.851851851851848</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="C42">
+        <v>59</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42" si="13">C42/B42</f>
+        <v>81.155433287482808</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>53.941908713692946</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="B44">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="C44">
+        <v>49</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>73.573573573573569</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>0.49</v>
+      </c>
+      <c r="C45">
+        <v>42</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ref="D45" si="14">C45/B45</f>
+        <v>85.714285714285722</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46">
+        <v>1.149</v>
+      </c>
+      <c r="C46">
+        <v>82</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>71.36640557006092</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D43" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B47">
+        <v>2.468</v>
+      </c>
+      <c r="C47">
+        <v>134</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>54.294975688816855</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>1.264</v>
+      </c>
+      <c r="C48">
+        <v>75</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48" si="15">C48/B48</f>
+        <v>59.335443037974684</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>60.386473429951693</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D50" t="e">
         <f t="shared" si="0"/>
@@ -1856,7 +1928,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D51" t="e">
         <f t="shared" si="0"/>
@@ -1865,7 +1937,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D52" t="e">
         <f t="shared" si="0"/>
@@ -1874,7 +1946,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D53" t="e">
         <f t="shared" si="0"/>
@@ -1883,7 +1955,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D54" t="e">
         <f t="shared" si="0"/>
@@ -1892,7 +1964,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D55" t="e">
         <f t="shared" si="0"/>
@@ -1901,7 +1973,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D56" t="e">
         <f t="shared" si="0"/>
@@ -1910,61 +1982,61 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D57" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D58" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D60" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D62" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D63" t="e">
         <f t="shared" si="0"/>
@@ -1973,7 +2045,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D64" t="e">
         <f t="shared" si="0"/>
@@ -1982,7 +2054,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D65" t="e">
         <f t="shared" si="0"/>
@@ -1991,7 +2063,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D66" t="e">
         <f t="shared" si="0"/>
@@ -2000,7 +2072,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D67" t="e">
         <f t="shared" si="0"/>
@@ -2009,7 +2081,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D68" t="e">
         <f t="shared" si="0"/>
@@ -2018,7 +2090,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D69" t="e">
         <f t="shared" si="0"/>
@@ -2027,7 +2099,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D70" t="e">
         <f t="shared" si="0"/>
@@ -2036,7 +2108,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D71" t="e">
         <f t="shared" si="0"/>
@@ -2045,7 +2117,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D72" t="e">
         <f t="shared" si="0"/>
@@ -2054,7 +2126,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D73" t="e">
         <f t="shared" si="0"/>
@@ -2063,7 +2135,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D74" t="e">
         <f t="shared" si="0"/>
@@ -2072,7 +2144,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D75" t="e">
         <f t="shared" si="0"/>
@@ -2081,7 +2153,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D76" t="e">
         <f t="shared" si="0"/>
@@ -2090,7 +2162,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D77" t="e">
         <f t="shared" si="0"/>
@@ -2099,7 +2171,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D78" t="e">
         <f t="shared" si="0"/>
@@ -2108,7 +2180,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D79" t="e">
         <f t="shared" si="0"/>
@@ -2117,7 +2189,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D80" t="e">
         <f t="shared" si="0"/>
@@ -2126,7 +2198,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D81" t="e">
         <f t="shared" si="0"/>
@@ -2135,7 +2207,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D82" t="e">
         <f t="shared" si="0"/>
@@ -2144,7 +2216,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D83" t="e">
         <f t="shared" si="0"/>
@@ -2153,7 +2225,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D84" t="e">
         <f t="shared" si="0"/>
@@ -2162,7 +2234,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D85" t="e">
         <f t="shared" si="0"/>
@@ -2171,7 +2243,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D86" t="e">
         <f t="shared" si="0"/>
@@ -2180,9 +2252,63 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D87" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D88" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D89" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D90" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D92" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D87" t="e">
+      <c r="D93" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
week 7 done ish
</commit_message>
<xml_diff>
--- a/data/Experiment/Raw/StomatalDensity.xlsx
+++ b/data/Experiment/Raw/StomatalDensity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/SeedlingMortality/data/Experiment/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9212CDA-6C66-2544-BB01-DEF367E9492F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B77E45-D2E4-E141-9704-E7718AE71D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22520" windowHeight="17120" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
@@ -1175,7 +1175,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A47:A49"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>